<commit_message>
research paper added and minor changes made in code
</commit_message>
<xml_diff>
--- a/docs/Classification Reports/decisiontree.xlsx
+++ b/docs/Classification Reports/decisiontree.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7320261437908496</v>
+        <v>0.6967741935483871</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7368421052631579</v>
+        <v>0.7448275862068966</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7344262295081967</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8472222222222222</v>
       </c>
       <c r="C3" t="n">
-        <v>0.732484076433121</v>
+        <v>0.8243243243243243</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7796610169491525</v>
+        <v>0.8356164383561645</v>
       </c>
       <c r="E3" t="n">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7905405405405406</v>
+        <v>0.7435897435897436</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8125</v>
+        <v>0.7682119205298014</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8013698630136987</v>
+        <v>0.7557003257328991</v>
       </c>
       <c r="E4" t="n">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.6896551724137931</v>
       </c>
       <c r="C5" t="n">
-        <v>0.782312925170068</v>
+        <v>0.6410256410256411</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7467532467532468</v>
+        <v>0.6644518272425251</v>
       </c>
       <c r="E5" t="n">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.765</v>
+        <v>0.7433333333333333</v>
       </c>
       <c r="C6" t="n">
-        <v>0.765</v>
+        <v>0.7433333333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>0.765</v>
+        <v>0.7433333333333333</v>
       </c>
       <c r="E6" t="n">
-        <v>0.765</v>
+        <v>0.7433333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -557,13 +557,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7675464329876095</v>
+        <v>0.7443103329435365</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7660347767165867</v>
+        <v>0.7445973680216658</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7655525890560736</v>
+        <v>0.7439421478328971</v>
       </c>
       <c r="E7" t="n">
         <v>600</v>
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7682319083789672</v>
+        <v>0.7438156752200134</v>
       </c>
       <c r="C8" t="n">
-        <v>0.765</v>
+        <v>0.7433333333333333</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7653492568216046</v>
+        <v>0.7430607785203568</v>
       </c>
       <c r="E8" t="n">
         <v>600</v>

</xml_diff>